<commit_message>
fix scenario result: sparse tree with large transmission cost
</commit_message>
<xml_diff>
--- a/result/comparision.xlsx
+++ b/result/comparision.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\k1759921\Documents\code\matlab\Energy-aware-Proactive-Caching\result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{02B9262F-A0E8-4C13-927A-49573A4D6FA6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4970"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14376" windowHeight="4968"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,14 +29,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="47">
   <si>
     <t>4,2,3</t>
   </si>
   <si>
-    <t>dense</t>
-  </si>
-  <si>
     <t>MILP</t>
   </si>
   <si>
@@ -111,13 +107,76 @@
   </si>
   <si>
     <t>4,1,(1,2,3)</t>
+  </si>
+  <si>
+    <t>sparse</t>
+  </si>
+  <si>
+    <t>dense+L</t>
+  </si>
+  <si>
+    <t>1,1,1</t>
+  </si>
+  <si>
+    <t>1,2,4</t>
+  </si>
+  <si>
+    <t>1,1,(2,3)</t>
+  </si>
+  <si>
+    <t>1,2,(2,3)</t>
+  </si>
+  <si>
+    <t>1,2,(3,4)</t>
+  </si>
+  <si>
+    <t>1,2,(1,3,4)</t>
+  </si>
+  <si>
+    <t>1,1,(2,3,4)</t>
+  </si>
+  <si>
+    <t>1,2,(1,2,3)</t>
+  </si>
+  <si>
+    <t>1,1,(1,2,3,4)</t>
+  </si>
+  <si>
+    <t>1,2,(1,2,3,4)</t>
+  </si>
+  <si>
+    <t>1,2,(1,2)</t>
+  </si>
+  <si>
+    <t>1,1,(1,2,3)</t>
+  </si>
+  <si>
+    <t>sparse_L</t>
+  </si>
+  <si>
+    <t>1,1,2</t>
+  </si>
+  <si>
+    <t>1,1,4</t>
+  </si>
+  <si>
+    <t>1,1,(1,3)</t>
+  </si>
+  <si>
+    <t>1,1,(1,2)</t>
+  </si>
+  <si>
+    <t>1,1,(1,2);6,2,4</t>
+  </si>
+  <si>
+    <t>3,1,(1,2);6,1,(1,3)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,13 +184,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -143,17 +214,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="好" xfId="1" builtinId="26"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -465,166 +539,336 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="3" width="10.26953125" customWidth="1"/>
+    <col min="2" max="3" width="10.21875" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" customWidth="1"/>
+    <col min="7" max="7" width="10.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
       </c>
       <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>18</v>
       </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>19</v>
       </c>
-      <c r="C7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>20</v>
       </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>21</v>
       </c>
-      <c r="C9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>22</v>
       </c>
-      <c r="C10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>23</v>
       </c>
-      <c r="C11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>13</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
         <v>24</v>
       </c>
-      <c r="C12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" t="s">
-        <v>25</v>
-      </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="D14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>